<commit_message>
security: replace real client data with sample data
- Remove Excel file with real client data from git tracking
- Create new Excel file with anonymized sample data
- Add .gitignore rules to prevent future real data commits
- Update README to mention sample data in Excel template
- Include Python script for regenerating sample data if needed
</commit_message>
<xml_diff>
--- a/monday_board_import.xlsx
+++ b/monday_board_import.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="ABS Shift Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Column Mapping" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Instructions" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,131 +493,131 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6:40 AM - 9:40 AM</t>
+          <t>06:30 AM - 10:00 AM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6:40 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9:40 AM</t>
+          <t>10:00 AM</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Smith, Tony</t>
+          <t>Sample Client A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Nolen, Carlos</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>TN - Memphis</t>
+          <t>MS - Jackson</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CHOICES Personal Care (T1019)</t>
+          <t>Meal Prep</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>$26.36</t>
+          <t>$30.12</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>$13.00</t>
+          <t>$24.51</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Open</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7:00 AM - 7:00 PM</t>
+          <t>09:30 AM - 15:15 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7:00 AM</t>
+          <t>09:30 AM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>15:15 PM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Smith, Bryce</t>
+          <t>Sample Client E</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Johnson, Sarah</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>TN - Nashville</t>
+          <t>AR - Little Rock</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Home Health Aide (HHA)</t>
+          <t>Personal Care</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>$28.50</t>
+          <t>$37.49</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>$15.00</t>
+          <t>$20.97</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Assigned</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8:00 AM - 12:00 PM</t>
+          <t>09:30 AM - 12:00 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8:00 AM</t>
+          <t>09:30 AM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -629,85 +627,89 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Davis, Mary</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>Sample Client B</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>David Brown</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TN - Knoxville</t>
+          <t>TN - Memphis</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Personal Care Services</t>
+          <t>Personal Care</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$25.00</t>
+          <t>$26.59</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>$12.50</t>
+          <t>$18.34</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Assigned</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2:00 PM - 6:00 PM</t>
+          <t>08:15 AM - 11:00 AM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>08:15 AM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Wilson, John</t>
+          <t>Sample Client B</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Brown, Michael</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>TN - Chattanooga</t>
+          <t>LA - New Orleans</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Companion Care</t>
+          <t>Personal Care</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>$22.00</t>
+          <t>$35.91</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>$11.00</t>
+          <t>$21.99</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -719,466 +721,912 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9:00 AM - 5:00 PM</t>
+          <t>10:30 AM - 12:45 PM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9:00 AM</t>
+          <t>10:30 AM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>12:45 PM</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Taylor, Lisa</t>
+          <t>Sample Client C</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Garcia, Maria</t>
+          <t>Amy Garcia</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TN - Memphis</t>
+          <t>LA - New Orleans</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Skilled Nursing</t>
+          <t>Companion Care</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>$35.00</t>
+          <t>$40.56</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>$18.00</t>
+          <t>$17.10</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>Assigned</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Column Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Monday.com Type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Shift date (YYYY-MM-DD format)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Full time range (e.g., "6:40 AM - 9:40 AM")</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Start time (e.g., "6:40 AM")</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>End time (e.g., "9:40 AM")</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>client</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Client name (e.g., "Smith, Tony")</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>employee</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>09:45 AM - 17:15 PM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Employee name (e.g., "Nolen, Carlos")</t>
+          <t>09:45 AM</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17:15 PM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sample Client C</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>David Brown</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TN - Memphis</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Companion Care</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>$44.70</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>$24.23</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>10:00 AM - 12:45 PM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Work location (e.g., "TN - Memphis")</t>
+          <t>10:00 AM</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12:45 PM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sample Client C</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Sarah Wilson</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TN - Memphis</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Companion Care</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>$29.12</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>$21.31</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Open</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>10:15 AM - 18:15 PM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Service/product type</t>
+          <t>10:15 AM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>18:15 PM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Sample Client E</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Mike Johnson</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>AR - Little Rock</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>$41.68</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>$21.26</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Open</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>bill_rate</t>
+          <t>2025-09-07</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>06:00 AM - 12:15 PM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Billing rate (e.g., "$26.36")</t>
+          <t>06:00 AM</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>12:15 PM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sample Client D</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mike Johnson</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>LA - New Orleans</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Respite Care</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>$41.51</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>$21.73</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Assigned</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>pay_rate</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>09:15 AM - 12:45 PM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pay rate (e.g., "$13.00")</t>
+          <t>09:15 AM</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12:45 PM</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Sample Client F</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sarah Wilson</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>LA - New Orleans</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Respite Care</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>$26.24</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>$23.50</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>10:15 AM - 17:30 PM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Shift status: Open (red), Assigned (green), Completed (blue)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Action</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Download this Excel file</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Save monday_board_import.xlsx to your computer</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Go to Monday.com</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Log into your Monday.com workspace</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Create new board</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Click "+" to create a new board</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Import from Excel</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Choose "Import from Excel" option</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Upload file</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Upload this Excel file</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Name the board</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Name it "ABS Shift Data"</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Map columns</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Use the Column Mapping sheet to set correct column types</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Set status colors</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Configure status column: Open=red, Assigned=green, Completed=blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Get board ID</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Copy the board ID from the URL and add to .env as MONDAY_BOARD_ID</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Test integration</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Run "npm run sync-monday" to test</t>
+          <t>10:15 AM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>17:30 PM</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Sample Client B</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tom Miller</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>AL - Birmingham</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Companion Care</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>$28.10</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>$23.10</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:15 AM - 13:00 PM</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10:15 AM</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>13:00 PM</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sample Client C</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>TN - Memphis</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>$26.41</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>$22.30</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:30 AM - 11:15 AM</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>11:15 AM</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sample Client D</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>TN - Memphis</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Companion Care</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>$39.34</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>$16.74</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-09-01</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:15 AM - 10:15 AM</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>07:15 AM</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10:15 AM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sample Client E</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Lisa Davis</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>AL - Birmingham</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>$41.13</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>$15.93</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:45 AM - 17:45 PM</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10:45 AM</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>17:45 PM</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Sample Client B</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>TN - Nashville</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Medication Management</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>$34.48</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>$17.70</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:00 AM - 11:30 AM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>08:00 AM</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11:30 AM</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sample Client C</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>AR - Little Rock</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Respite Care</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>$31.14</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>$19.80</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:30 AM - 13:30 PM</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>13:30 PM</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sample Client B</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>MS - Jackson</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Personal Care</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>$28.43</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>$22.98</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-09-21</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:15 AM - 15:00 PM</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>08:15 AM</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>15:00 PM</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Sample Client A</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>LA - New Orleans</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Medication Management</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>$25.97</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>$18.31</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:15 AM - 14:45 PM</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>09:15 AM</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>14:45 PM</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Sample Client B</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Lisa Davis</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>MS - Jackson</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Companion Care</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>$35.07</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>$23.90</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:00 AM - 14:15 PM</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>09:00 AM</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>14:15 PM</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Sample Client C</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Tom Miller</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>LA - New Orleans</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Medication Management</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>$44.68</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>$16.61</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Completed</t>
         </is>
       </c>
     </row>

</xml_diff>